<commit_message>
Added Recruitment Sheet Instructions
</commit_message>
<xml_diff>
--- a/docs/swing-weighting-exercise.xlsx
+++ b/docs/swing-weighting-exercise.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="7470" windowHeight="2670"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="7470" windowHeight="2670" firstSheet="2" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Meta" sheetId="1" r:id="rId1"/>
@@ -342,6 +342,8 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -351,8 +353,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -436,7 +436,7 @@
         <a:p>
           <a:r>
             <a:rPr lang="en-US" sz="1100"/>
-            <a:t>1) Rank each of the the rows</a:t>
+            <a:t>1) Rank each of the rows</a:t>
           </a:r>
           <a:r>
             <a:rPr lang="en-US" sz="1100" baseline="0"/>
@@ -620,7 +620,7 @@
         <a:p>
           <a:r>
             <a:rPr lang="en-US" sz="1100"/>
-            <a:t>2) Rank each of the the rows</a:t>
+            <a:t>2) Rank each of the rows</a:t>
           </a:r>
           <a:r>
             <a:rPr lang="en-US" sz="1100" baseline="0"/>
@@ -764,7 +764,7 @@
         <a:p>
           <a:r>
             <a:rPr lang="en-US" sz="1100"/>
-            <a:t>2) Rank each of the the rows</a:t>
+            <a:t>2) Rank each of the rows</a:t>
           </a:r>
           <a:r>
             <a:rPr lang="en-US" sz="1100" baseline="0"/>
@@ -923,7 +923,7 @@
         <a:p>
           <a:r>
             <a:rPr lang="en-US" sz="1600"/>
-            <a:t>1) Rank each of the the rows</a:t>
+            <a:t>1) Rank each of the rows</a:t>
           </a:r>
           <a:r>
             <a:rPr lang="en-US" sz="1600" baseline="0"/>
@@ -1309,8 +1309,8 @@
   </sheetPr>
   <dimension ref="A1:B17"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1341,24 +1341,24 @@
       <c r="B3" s="18"/>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="20"/>
-      <c r="B4" s="20"/>
+      <c r="A4" s="22"/>
+      <c r="B4" s="22"/>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="19" t="s">
+      <c r="A5" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="19"/>
+      <c r="B5" s="21"/>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="21" t="s">
+      <c r="A6" s="23" t="s">
         <v>36</v>
       </c>
-      <c r="B6" s="21"/>
+      <c r="B6" s="23"/>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" s="22"/>
-      <c r="B17" s="23"/>
+      <c r="A17" s="19"/>
+      <c r="B17" s="20"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -1382,7 +1382,7 @@
   </sheetPr>
   <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
@@ -1650,7 +1650,7 @@
   </sheetPr>
   <dimension ref="A1:G6"/>
   <sheetViews>
-    <sheetView zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="78" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="78" workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
fix number of sheets
</commit_message>
<xml_diff>
--- a/docs/swing-weighting-exercise.xlsx
+++ b/docs/swing-weighting-exercise.xlsx
@@ -1,23 +1,29 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sreynolds\Documents\GitHub\PSPAP-Reboot\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="7476" windowHeight="2676"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="7470" windowHeight="2670" firstSheet="2" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Meta" sheetId="1" r:id="rId1"/>
-    <sheet name="Abundance" sheetId="3" r:id="rId2"/>
-    <sheet name="Trend" sheetId="2" r:id="rId3"/>
-    <sheet name="Fundamental Objectives" sheetId="4" r:id="rId4"/>
+    <sheet name="Recruitment" sheetId="5" r:id="rId2"/>
+    <sheet name="Abundance" sheetId="3" r:id="rId3"/>
+    <sheet name="Trend" sheetId="2" r:id="rId4"/>
+    <sheet name="Fundamental Objectives" sheetId="4" r:id="rId5"/>
   </sheets>
   <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="41">
   <si>
     <t>Name:</t>
   </si>
@@ -38,6 +44,25 @@
   </si>
   <si>
     <t>Scenario</t>
+  </si>
+  <si>
+    <t>Probablity to detect age-1 
+recruits given recruitment</t>
+  </si>
+  <si>
+    <t>Probability of having sufficient catch to estimate occupancy</t>
+  </si>
+  <si>
+    <t>Probability to detect recruitment that occurred is 0</t>
+  </si>
+  <si>
+    <t>Probability of having enough catch to run the analysis is 0</t>
+  </si>
+  <si>
+    <t>Probability to detect recruitment that occurred is 100</t>
+  </si>
+  <si>
+    <t>Probability of having enough catch to run the analysis is 100</t>
   </si>
   <si>
     <t>Monitoring program estimates no pallid sturgeon population model inputs</t>
@@ -173,7 +198,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -351,6 +376,165 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>60960</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>619125</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>66676</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="TextBox 1"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="38100" y="3061335"/>
+          <a:ext cx="5762625" cy="1339216"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="bg1">
+            <a:lumMod val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1"/>
+            <a:t>Instructions.</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>1) Rank each of the rows</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t> with the baseline the worst rank. For rankings 1 is best and 2 is the worst.</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>2) Assign the scenario that you ranked 1 with a value of 100</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US">
+            <a:effectLst/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>3) Assign a value, from 0 to 100, to the remaining scenarios (0 is worst and 100 is the best).</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US">
+            <a:effectLst/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>** Values do not need to sum to 100 but do need to increase with ranking.</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US">
+            <a:effectLst/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>** Do not change the shaded cells in the table above</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t> </a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US">
+            <a:effectLst/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
       <xdr:colOff>38101</xdr:colOff>
       <xdr:row>4</xdr:row>
       <xdr:rowOff>76200</xdr:rowOff>
@@ -490,7 +674,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -674,7 +858,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -876,7 +1060,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -911,7 +1095,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1125,15 +1309,15 @@
   </sheetPr>
   <dimension ref="A1:B17"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.88671875" style="17"/>
-    <col min="2" max="2" width="65.109375" style="17" customWidth="1"/>
-    <col min="3" max="16384" width="8.88671875" style="17"/>
+    <col min="1" max="1" width="8.85546875" style="17"/>
+    <col min="2" max="2" width="65.140625" style="17" customWidth="1"/>
+    <col min="3" max="16384" width="8.85546875" style="17"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -1168,7 +1352,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="23" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="B6" s="23"/>
     </row>
@@ -1196,48 +1380,47 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+    <sheetView topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14" customWidth="1"/>
-    <col min="2" max="2" width="24.6640625" customWidth="1"/>
-    <col min="3" max="3" width="27.88671875" customWidth="1"/>
-    <col min="4" max="4" width="15.5546875" customWidth="1"/>
-    <col min="5" max="5" width="17.44140625" customWidth="1"/>
-    <col min="6" max="6" width="17.109375" customWidth="1"/>
+    <col min="1" max="1" width="21.140625" customWidth="1"/>
+    <col min="2" max="2" width="25.28515625" customWidth="1"/>
+    <col min="3" max="3" width="21" customWidth="1"/>
+    <col min="4" max="4" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="2" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A1" s="13" t="s">
+    <row r="1" spans="1:5" ht="63" x14ac:dyDescent="0.25">
+      <c r="A1" s="12" t="s">
         <v>6</v>
       </c>
       <c r="B1" s="13" t="s">
-        <v>29</v>
+        <v>7</v>
       </c>
       <c r="C1" s="13" t="s">
-        <v>33</v>
-      </c>
-      <c r="D1" s="15" t="s">
-        <v>15</v>
-      </c>
-      <c r="E1" s="15" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" ht="62.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+      <c r="D1" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="E1" s="14" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
         <v>4</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>27</v>
+        <v>9</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>31</v>
+        <v>10</v>
       </c>
       <c r="D2" s="7">
         <v>3</v>
@@ -1246,33 +1429,32 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="54.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="63" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
-        <v>29</v>
+        <v>7</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>28</v>
+        <v>11</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="D3" s="5"/>
-      <c r="E3" s="5"/>
-    </row>
-    <row r="4" spans="1:5" ht="63" customHeight="1" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+      <c r="D3" s="4"/>
+      <c r="E3" s="4"/>
+    </row>
+    <row r="4" spans="1:5" ht="63" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
-        <v>33</v>
+        <v>8</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>27</v>
+        <v>9</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>32</v>
-      </c>
-      <c r="D4" s="5"/>
-      <c r="E4" s="5"/>
-    </row>
-    <row r="5" spans="1:5" ht="55.5" customHeight="1" x14ac:dyDescent="0.25"/>
+        <v>12</v>
+      </c>
+      <c r="D4" s="4"/>
+      <c r="E4" s="4"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup fitToHeight="0" orientation="landscape" verticalDpi="599" r:id="rId1"/>
@@ -1285,48 +1467,48 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.109375" customWidth="1"/>
-    <col min="2" max="2" width="25.44140625" customWidth="1"/>
-    <col min="3" max="3" width="28.88671875" customWidth="1"/>
-    <col min="4" max="4" width="14.44140625" customWidth="1"/>
-    <col min="5" max="5" width="14.88671875" customWidth="1"/>
-    <col min="6" max="6" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14" customWidth="1"/>
+    <col min="2" max="2" width="24.7109375" customWidth="1"/>
+    <col min="3" max="3" width="27.85546875" customWidth="1"/>
+    <col min="4" max="4" width="15.5703125" customWidth="1"/>
+    <col min="5" max="5" width="17.42578125" customWidth="1"/>
+    <col min="6" max="6" width="17.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A1" s="12" t="s">
+    <row r="1" spans="1:5" s="2" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A1" s="13" t="s">
         <v>6</v>
       </c>
       <c r="B1" s="13" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C1" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="D1" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="D1" s="14" t="s">
-        <v>15</v>
-      </c>
-      <c r="E1" s="14" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" ht="95.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E1" s="15" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="62.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="11" t="s">
-        <v>25</v>
+      <c r="B2" s="6" t="s">
+        <v>33</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>24</v>
+        <v>37</v>
       </c>
       <c r="D2" s="7">
         <v>3</v>
@@ -1335,39 +1517,36 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="100.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="54.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="B3" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="B3" s="10" t="s">
-        <v>26</v>
-      </c>
       <c r="C3" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="D3" s="4"/>
-      <c r="E3" s="4"/>
-    </row>
-    <row r="4" spans="1:5" ht="86.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>37</v>
+      </c>
+      <c r="D3" s="5"/>
+      <c r="E3" s="5"/>
+    </row>
+    <row r="4" spans="1:5" ht="63" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
-        <v>21</v>
-      </c>
-      <c r="B4" s="11" t="s">
-        <v>25</v>
+        <v>39</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>33</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="D4" s="4"/>
-      <c r="E4" s="4"/>
-    </row>
-    <row r="5" spans="1:5" ht="100.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="11" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="D11" s="3"/>
-    </row>
+        <v>38</v>
+      </c>
+      <c r="D4" s="5"/>
+      <c r="E4" s="5"/>
+    </row>
+    <row r="5" spans="1:5" ht="55.5" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup scale="95" fitToHeight="0" orientation="landscape" verticalDpi="599" r:id="rId1"/>
+  <pageSetup fitToHeight="0" orientation="landscape" verticalDpi="599" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
 </file>
@@ -1377,44 +1556,136 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
+  <dimension ref="A1:E11"/>
+  <sheetViews>
+    <sheetView topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I5" sqref="I5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15.140625" customWidth="1"/>
+    <col min="2" max="2" width="25.42578125" customWidth="1"/>
+    <col min="3" max="3" width="28.85546875" customWidth="1"/>
+    <col min="4" max="4" width="14.42578125" customWidth="1"/>
+    <col min="5" max="5" width="14.85546875" customWidth="1"/>
+    <col min="6" max="6" width="13.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A1" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="C1" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="D1" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="E1" s="14" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="95.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="D2" s="7">
+        <v>3</v>
+      </c>
+      <c r="E2" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="100.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="B3" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="D3" s="4"/>
+      <c r="E3" s="4"/>
+    </row>
+    <row r="4" spans="1:5" ht="86.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="B4" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="C4" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="D4" s="4"/>
+      <c r="E4" s="4"/>
+    </row>
+    <row r="5" spans="1:5" ht="100.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D11" s="3"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup scale="95" fitToHeight="0" orientation="landscape" verticalDpi="599" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
   <dimension ref="A1:G6"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="78" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="78" workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18" style="2" customWidth="1"/>
-    <col min="2" max="2" width="20.88671875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="24.44140625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="19.88671875" style="1" customWidth="1"/>
-    <col min="5" max="5" width="23.33203125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="16.6640625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="20.5546875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="20.85546875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="24.42578125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="19.85546875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="23.28515625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="16.7109375" style="1" customWidth="1"/>
+    <col min="7" max="7" width="20.5703125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="67.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" ht="67.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="15" t="s">
         <v>6</v>
       </c>
       <c r="B1" s="15" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="C1" s="15" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="D1" s="15" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="E1" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="F1" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="G1" s="14" t="s">
         <v>20</v>
-      </c>
-      <c r="F1" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="G1" s="14" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="96" customHeight="1" x14ac:dyDescent="0.25">
@@ -1422,16 +1693,16 @@
         <v>4</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="F2" s="7">
         <v>5</v>
@@ -1442,76 +1713,76 @@
     </row>
     <row r="3" spans="1:7" ht="98.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="15" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="B3" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="D3" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="C3" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="D3" s="8" t="s">
-        <v>7</v>
-      </c>
       <c r="E3" s="8" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="F3" s="5"/>
       <c r="G3" s="5"/>
     </row>
-    <row r="4" spans="1:7" ht="96.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" ht="96.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="B4" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="B4" s="8" t="s">
-        <v>12</v>
-      </c>
       <c r="C4" s="9" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="E4" s="8" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="F4" s="5"/>
       <c r="G4" s="5"/>
     </row>
     <row r="5" spans="1:7" ht="100.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="15" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="D5" s="9" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="E5" s="8" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="F5" s="5"/>
       <c r="G5" s="5"/>
     </row>
     <row r="6" spans="1:7" ht="100.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="15" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="E6" s="9" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="F6" s="5"/>
       <c r="G6" s="5"/>

</xml_diff>

<commit_message>
Using newly synced database
</commit_message>
<xml_diff>
--- a/docs/swing-weighting-exercise.xlsx
+++ b/docs/swing-weighting-exercise.xlsx
@@ -9,21 +9,20 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="7470" windowHeight="2670" firstSheet="2" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="7470" windowHeight="2670" firstSheet="1" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Meta" sheetId="1" r:id="rId1"/>
-    <sheet name="Recruitment" sheetId="5" r:id="rId2"/>
-    <sheet name="Abundance" sheetId="3" r:id="rId3"/>
-    <sheet name="Trend" sheetId="2" r:id="rId4"/>
-    <sheet name="Fundamental Objectives" sheetId="4" r:id="rId5"/>
+    <sheet name="Abundance" sheetId="3" r:id="rId2"/>
+    <sheet name="Trend" sheetId="2" r:id="rId3"/>
+    <sheet name="Fundamental Objectives" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="35">
   <si>
     <t>Name:</t>
   </si>
@@ -44,25 +43,6 @@
   </si>
   <si>
     <t>Scenario</t>
-  </si>
-  <si>
-    <t>Probablity to detect age-1 
-recruits given recruitment</t>
-  </si>
-  <si>
-    <t>Probability of having sufficient catch to estimate occupancy</t>
-  </si>
-  <si>
-    <t>Probability to detect recruitment that occurred is 0</t>
-  </si>
-  <si>
-    <t>Probability of having enough catch to run the analysis is 0</t>
-  </si>
-  <si>
-    <t>Probability to detect recruitment that occurred is 100</t>
-  </si>
-  <si>
-    <t>Probability of having enough catch to run the analysis is 100</t>
   </si>
   <si>
     <t>Monitoring program estimates no pallid sturgeon population model inputs</t>
@@ -376,165 +356,6 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>38100</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>60960</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>619125</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>66676</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="2" name="TextBox 1"/>
-        <xdr:cNvSpPr txBox="1"/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="38100" y="3061335"/>
-          <a:ext cx="5762625" cy="1339216"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:schemeClr val="bg1">
-            <a:lumMod val="95000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:ln w="9525" cmpd="sng">
-          <a:solidFill>
-            <a:schemeClr val="tx1"/>
-          </a:solidFill>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="dk1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" b="1"/>
-            <a:t>Instructions.</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100"/>
-            <a:t>1) Rank each of the rows</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" baseline="0"/>
-            <a:t> with the baseline the worst rank. For rankings 1 is best and 2 is the worst.</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="dk1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>2) Assign the scenario that you ranked 1 with a value of 100</a:t>
-          </a:r>
-          <a:endParaRPr lang="en-US">
-            <a:effectLst/>
-          </a:endParaRPr>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="dk1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>3) Assign a value, from 0 to 100, to the remaining scenarios (0 is worst and 100 is the best).</a:t>
-          </a:r>
-          <a:endParaRPr lang="en-US">
-            <a:effectLst/>
-          </a:endParaRPr>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" b="1" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="dk1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>** Values do not need to sum to 100 but do need to increase with ranking.</a:t>
-          </a:r>
-          <a:endParaRPr lang="en-US">
-            <a:effectLst/>
-          </a:endParaRPr>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" b="1" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="dk1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>** Do not change the shaded cells in the table above</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="dk1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t> </a:t>
-          </a:r>
-          <a:endParaRPr lang="en-US">
-            <a:effectLst/>
-          </a:endParaRPr>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
-</file>
-
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>0</xdr:col>
       <xdr:colOff>38101</xdr:colOff>
       <xdr:row>4</xdr:row>
       <xdr:rowOff>76200</xdr:rowOff>
@@ -674,7 +495,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -858,7 +679,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -1352,7 +1173,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="23" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="B6" s="23"/>
     </row>
@@ -1380,96 +1201,9 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:E4"/>
-  <sheetViews>
-    <sheetView topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="21.140625" customWidth="1"/>
-    <col min="2" max="2" width="25.28515625" customWidth="1"/>
-    <col min="3" max="3" width="21" customWidth="1"/>
-    <col min="4" max="4" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.28515625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" ht="63" x14ac:dyDescent="0.25">
-      <c r="A1" s="12" t="s">
-        <v>6</v>
-      </c>
-      <c r="B1" s="13" t="s">
-        <v>7</v>
-      </c>
-      <c r="C1" s="13" t="s">
-        <v>8</v>
-      </c>
-      <c r="D1" s="14" t="s">
-        <v>21</v>
-      </c>
-      <c r="E1" s="14" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A2" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="C2" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="D2" s="7">
-        <v>3</v>
-      </c>
-      <c r="E2" s="7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" ht="63" x14ac:dyDescent="0.25">
-      <c r="A3" s="13" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="C3" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="D3" s="4"/>
-      <c r="E3" s="4"/>
-    </row>
-    <row r="4" spans="1:5" ht="63" x14ac:dyDescent="0.25">
-      <c r="A4" s="13" t="s">
-        <v>8</v>
-      </c>
-      <c r="B4" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="D4" s="4"/>
-      <c r="E4" s="4"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup fitToHeight="0" orientation="landscape" verticalDpi="599" r:id="rId1"/>
-  <drawing r:id="rId2"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
-    <pageSetUpPr fitToPage="1"/>
-  </sheetPr>
   <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
@@ -1488,16 +1222,16 @@
         <v>6</v>
       </c>
       <c r="B1" s="13" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="C1" s="13" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="D1" s="15" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="E1" s="15" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="62.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1505,10 +1239,10 @@
         <v>4</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="D2" s="7">
         <v>3</v>
@@ -1519,26 +1253,26 @@
     </row>
     <row r="3" spans="1:5" ht="54.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="D3" s="5"/>
       <c r="E3" s="5"/>
     </row>
     <row r="4" spans="1:5" ht="63" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="D4" s="5"/>
       <c r="E4" s="5"/>
@@ -1551,7 +1285,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
@@ -1577,16 +1311,16 @@
         <v>6</v>
       </c>
       <c r="B1" s="13" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="C1" s="13" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="D1" s="14" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="E1" s="14" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="95.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1594,10 +1328,10 @@
         <v>4</v>
       </c>
       <c r="B2" s="11" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="D2" s="7">
         <v>3</v>
@@ -1608,26 +1342,26 @@
     </row>
     <row r="3" spans="1:5" ht="100.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="D3" s="4"/>
       <c r="E3" s="4"/>
     </row>
     <row r="4" spans="1:5" ht="86.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="D4" s="4"/>
       <c r="E4" s="4"/>
@@ -1643,14 +1377,14 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:G6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="78" workbookViewId="0">
+    <sheetView topLeftCell="A8" zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="78" workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
@@ -1670,22 +1404,22 @@
         <v>6</v>
       </c>
       <c r="B1" s="15" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="C1" s="15" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="D1" s="15" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="E1" s="15" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="F1" s="14" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="G1" s="14" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="96" customHeight="1" x14ac:dyDescent="0.25">
@@ -1693,16 +1427,16 @@
         <v>4</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="F2" s="7">
         <v>5</v>
@@ -1713,76 +1447,76 @@
     </row>
     <row r="3" spans="1:7" ht="98.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="15" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="F3" s="5"/>
       <c r="G3" s="5"/>
     </row>
     <row r="4" spans="1:7" ht="96.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="15" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="E4" s="8" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="F4" s="5"/>
       <c r="G4" s="5"/>
     </row>
     <row r="5" spans="1:7" ht="100.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="15" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="D5" s="9" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="E5" s="8" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="F5" s="5"/>
       <c r="G5" s="5"/>
     </row>
     <row r="6" spans="1:7" ht="100.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="15" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="E6" s="9" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="F6" s="5"/>
       <c r="G6" s="5"/>

</xml_diff>

<commit_message>
fig & swing weighting cost update
</commit_message>
<xml_diff>
--- a/docs/swing-weighting-exercise.xlsx
+++ b/docs/swing-weighting-exercise.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="45">
   <si>
     <t>Name:</t>
   </si>
@@ -72,9 +72,6 @@
   </si>
   <si>
     <t>Rank (1-3)</t>
-  </si>
-  <si>
-    <t>Rank (1-5)</t>
   </si>
   <si>
     <t xml:space="preserve">Quantify PS recruitment to age-1 </t>
@@ -196,6 +193,18 @@
   </si>
   <si>
     <t>Abundance estimates have the least utility of 0 (least useful estimates; e.g., estimates have poor  precision and high bias)</t>
+  </si>
+  <si>
+    <t>Minimize Cost</t>
+  </si>
+  <si>
+    <t>Monitoring  program is within allotted budget, but is the most expensive.</t>
+  </si>
+  <si>
+    <t>Monitoring  program is the least expensive and is within allotted budget.</t>
+  </si>
+  <si>
+    <t>Rank (1-6)</t>
   </si>
 </sst>
 </file>
@@ -301,7 +310,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -361,6 +370,19 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -534,19 +556,7 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t>t</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" b="0" i="0">
-              <a:solidFill>
-                <a:schemeClr val="dk1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>he baseline,</a:t>
+            <a:t>the baseline,</a:t>
           </a:r>
           <a:r>
             <a:rPr lang="en-US" sz="1100" b="0" i="0" baseline="0">
@@ -1974,15 +1984,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>25400</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>78739</xdr:rowOff>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>158113</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>1349376</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>79375</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>1387475</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>174624</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -1991,8 +2001,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="25400" y="8524239"/>
-          <a:ext cx="9070976" cy="1715136"/>
+          <a:off x="0" y="8174988"/>
+          <a:ext cx="11912600" cy="1731011"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2038,7 +2048,7 @@
           </a:r>
           <a:r>
             <a:rPr lang="en-US" sz="1600" baseline="0"/>
-            <a:t> with the baseline the worst rank. For rankings 1 is best and 5 is the worst. </a:t>
+            <a:t> with the baseline the worst rank. For rankings 1 is best and 6 is the worst. </a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -2463,7 +2473,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="24" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B6" s="24"/>
     </row>
@@ -2513,10 +2523,10 @@
         <v>6</v>
       </c>
       <c r="B1" s="11" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C1" s="11" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D1" s="13" t="s">
         <v>15</v>
@@ -2530,10 +2540,10 @@
         <v>4</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D2" s="5">
         <v>3</v>
@@ -2544,26 +2554,26 @@
     </row>
     <row r="3" spans="1:5" ht="54.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="11" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D3" s="19"/>
       <c r="E3" s="19"/>
     </row>
     <row r="4" spans="1:5" ht="63" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="11" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D4" s="19"/>
       <c r="E4" s="19"/>
@@ -2603,10 +2613,10 @@
         <v>6</v>
       </c>
       <c r="B1" s="11" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C1" s="11" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D1" s="12" t="s">
         <v>15</v>
@@ -2620,10 +2630,10 @@
         <v>4</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D2" s="5">
         <v>3</v>
@@ -2634,26 +2644,26 @@
     </row>
     <row r="3" spans="1:5" ht="100.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="11" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D3" s="20"/>
       <c r="E3" s="20"/>
     </row>
     <row r="4" spans="1:5" ht="86.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="11" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D4" s="20"/>
       <c r="E4" s="20"/>
@@ -2691,10 +2701,10 @@
         <v>6</v>
       </c>
       <c r="B1" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1" s="11" t="s">
         <v>35</v>
-      </c>
-      <c r="C1" s="11" t="s">
-        <v>36</v>
       </c>
       <c r="D1" s="13" t="s">
         <v>15</v>
@@ -2708,10 +2718,10 @@
         <v>4</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D2" s="5">
         <v>3</v>
@@ -2722,26 +2732,26 @@
     </row>
     <row r="3" spans="1:8" ht="72" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="11" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D3" s="19"/>
       <c r="E3" s="19"/>
     </row>
     <row r="4" spans="1:8" ht="72" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="B4" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="B4" s="4" t="s">
-        <v>37</v>
-      </c>
       <c r="C4" s="8" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D4" s="19"/>
       <c r="E4" s="19"/>
@@ -2762,10 +2772,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="78" workbookViewId="0">
-      <selection activeCell="N5" sqref="N5"/>
+      <selection activeCell="M3" sqref="M3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2775,34 +2785,38 @@
     <col min="3" max="3" width="24.42578125" style="1" customWidth="1"/>
     <col min="4" max="4" width="23.42578125" style="1" customWidth="1"/>
     <col min="5" max="5" width="25.7109375" style="1" customWidth="1"/>
-    <col min="6" max="6" width="16.7109375" style="1" customWidth="1"/>
-    <col min="7" max="7" width="20.5703125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="20.28515625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="16.7109375" style="1" customWidth="1"/>
+    <col min="8" max="8" width="20.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="90" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" ht="90" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="13" t="s">
         <v>6</v>
       </c>
       <c r="B1" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="D1" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="C1" s="13" t="s">
-        <v>34</v>
-      </c>
-      <c r="D1" s="13" t="s">
+      <c r="E1" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="E1" s="13" t="s">
-        <v>19</v>
-      </c>
       <c r="F1" s="12" t="s">
-        <v>16</v>
+        <v>41</v>
       </c>
       <c r="G1" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="H1" s="12" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="90" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" ht="90" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
         <v>4</v>
       </c>
@@ -2810,7 +2824,7 @@
         <v>12</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D2" s="6" t="s">
         <v>7</v>
@@ -2818,22 +2832,25 @@
       <c r="E2" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="F2" s="5">
-        <v>5</v>
+      <c r="F2" s="25" t="s">
+        <v>42</v>
       </c>
       <c r="G2" s="5">
+        <v>6</v>
+      </c>
+      <c r="H2" s="5">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="90" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" ht="90" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B3" s="7" t="s">
         <v>13</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D3" s="6" t="s">
         <v>7</v>
@@ -2841,12 +2858,15 @@
       <c r="E3" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="F3" s="19"/>
+      <c r="F3" s="25" t="s">
+        <v>42</v>
+      </c>
       <c r="G3" s="19"/>
+      <c r="H3" s="19"/>
     </row>
-    <row r="4" spans="1:7" ht="90" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" ht="90" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B4" s="6" t="s">
         <v>12</v>
@@ -2860,18 +2880,21 @@
       <c r="E4" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="F4" s="19"/>
+      <c r="F4" s="25" t="s">
+        <v>42</v>
+      </c>
       <c r="G4" s="19"/>
+      <c r="H4" s="19"/>
     </row>
-    <row r="5" spans="1:7" ht="89.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" ht="89.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="13" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B5" s="6" t="s">
         <v>12</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D5" s="7" t="s">
         <v>10</v>
@@ -2879,18 +2902,21 @@
       <c r="E5" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="F5" s="19"/>
+      <c r="F5" s="25" t="s">
+        <v>42</v>
+      </c>
       <c r="G5" s="19"/>
+      <c r="H5" s="19"/>
     </row>
-    <row r="6" spans="1:7" ht="90.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" ht="90.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="13" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B6" s="6" t="s">
         <v>12</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D6" s="6" t="s">
         <v>7</v>
@@ -2898,13 +2924,38 @@
       <c r="E6" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="F6" s="19"/>
+      <c r="F6" s="25" t="s">
+        <v>42</v>
+      </c>
       <c r="G6" s="19"/>
+      <c r="H6" s="19"/>
+    </row>
+    <row r="7" spans="1:8" ht="90.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="F7" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="G7" s="27"/>
+      <c r="H7" s="28"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="YPK0otvCxu0otaSi0DRukvIzJ3cHYtSZUQb33emO1PLLfEeAPHxawtdzJWM0qwz5f9ViQHqRIli3979sVlHAxA==" saltValue="TKL6rIhcRe4hkJ0eCaTpsg==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="6NBnJ549xPb2yJ1c25tG6y2PcQ1mc15EhajLRLMYeJeA4RXvlzoq1oVW6ff/T+kkWyWjVgFl/AxOiyqA+qhFRQ==" saltValue="OWBv6YKgfC6MHXnMcY+7zg==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <dataValidations count="1">
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F3:F6">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G3:G6">
       <formula1>1</formula1>
       <formula2>4</formula2>
     </dataValidation>

</xml_diff>